<commit_message>
Finish adding Derbyshire stations
</commit_message>
<xml_diff>
--- a/lists/fire-data.xlsx
+++ b/lists/fire-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="13785" windowHeight="11895"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="13785" windowHeight="11895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fire-authority" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="538">
   <si>
     <t>name</t>
   </si>
@@ -1432,6 +1432,204 @@
   </si>
   <si>
     <t>government-domain?</t>
+  </si>
+  <si>
+    <t>Alfreton Community Fire Station</t>
+  </si>
+  <si>
+    <t>DE55 7AD</t>
+  </si>
+  <si>
+    <t>Ascot Drive Community Fire Station</t>
+  </si>
+  <si>
+    <t>DE24 8GZ</t>
+  </si>
+  <si>
+    <t>Ashbourne Fire Station</t>
+  </si>
+  <si>
+    <t>DE6 1FN</t>
+  </si>
+  <si>
+    <t>Bakewell Fire Station</t>
+  </si>
+  <si>
+    <t>DE45 1DA</t>
+  </si>
+  <si>
+    <t>Belper Fire Station</t>
+  </si>
+  <si>
+    <t>DE56 1BE</t>
+  </si>
+  <si>
+    <t>Bolsover Fire Station</t>
+  </si>
+  <si>
+    <t>S44 6HF</t>
+  </si>
+  <si>
+    <t>Bradwell Fire Station</t>
+  </si>
+  <si>
+    <t>S33 9JG</t>
+  </si>
+  <si>
+    <t>Buxton Fire &amp; Rescue Centre</t>
+  </si>
+  <si>
+    <t>SK17 9RZ</t>
+  </si>
+  <si>
+    <t>Chapel-en-le Frith Fire Station</t>
+  </si>
+  <si>
+    <t>SK23 0LX</t>
+  </si>
+  <si>
+    <t>Chesterfield Community Fire Station</t>
+  </si>
+  <si>
+    <t>S40 2WH</t>
+  </si>
+  <si>
+    <t>Clay Cross Fire Station</t>
+  </si>
+  <si>
+    <t>S45 9JQ</t>
+  </si>
+  <si>
+    <t>Clowne Fire Station</t>
+  </si>
+  <si>
+    <t>S43 4LS</t>
+  </si>
+  <si>
+    <t>Crich Fire Station</t>
+  </si>
+  <si>
+    <t>DE4 5DE</t>
+  </si>
+  <si>
+    <t>Derbyshire Fire &amp; Rescue Service HQ</t>
+  </si>
+  <si>
+    <t>DE23 6EH</t>
+  </si>
+  <si>
+    <t>Dronfield Fire Station</t>
+  </si>
+  <si>
+    <t>S18 1ST</t>
+  </si>
+  <si>
+    <t>Duffield Fire Station</t>
+  </si>
+  <si>
+    <t>DE56 4FQ</t>
+  </si>
+  <si>
+    <t>Glossop Fire Station</t>
+  </si>
+  <si>
+    <t>SK13 8LG</t>
+  </si>
+  <si>
+    <t>Hathersage Fire Station</t>
+  </si>
+  <si>
+    <t>S32 1DU</t>
+  </si>
+  <si>
+    <t>Heanor Fire Station</t>
+  </si>
+  <si>
+    <t>DE75 7DT</t>
+  </si>
+  <si>
+    <t>Ilkeston Community Fire Station</t>
+  </si>
+  <si>
+    <t>DE7 5EZ</t>
+  </si>
+  <si>
+    <t>Kingsway Fire Station</t>
+  </si>
+  <si>
+    <t>DE22 3LY</t>
+  </si>
+  <si>
+    <t>Long Eaton Fire Station</t>
+  </si>
+  <si>
+    <t>NG10 1BD</t>
+  </si>
+  <si>
+    <t>Matlock Fire Station</t>
+  </si>
+  <si>
+    <t>DE4 3DQ</t>
+  </si>
+  <si>
+    <t>Melbourne Fire Station</t>
+  </si>
+  <si>
+    <t>DE73 1DY</t>
+  </si>
+  <si>
+    <t>New Mills Fire Station</t>
+  </si>
+  <si>
+    <t>SK22 4JF</t>
+  </si>
+  <si>
+    <t>Nottingham Road Community Fire Station</t>
+  </si>
+  <si>
+    <t>DE21 6FP</t>
+  </si>
+  <si>
+    <t>Ripley Fire Station</t>
+  </si>
+  <si>
+    <t>DE5 3HR</t>
+  </si>
+  <si>
+    <t>Shirebrook Fire Station</t>
+  </si>
+  <si>
+    <t>NG20 8TY</t>
+  </si>
+  <si>
+    <t>Staveley Fire Station</t>
+  </si>
+  <si>
+    <t>S43 3PG</t>
+  </si>
+  <si>
+    <t>Swadlincote Fire Station</t>
+  </si>
+  <si>
+    <t>DE11 0AE</t>
+  </si>
+  <si>
+    <t>Whaley Bridge Fire Station</t>
+  </si>
+  <si>
+    <t>SK23 7HP</t>
+  </si>
+  <si>
+    <t>Wirksworth Fire Station</t>
+  </si>
+  <si>
+    <t>DE4 4FG</t>
+  </si>
+  <si>
+    <t>day staffing</t>
+  </si>
+  <si>
+    <t>Day staffing</t>
   </si>
 </sst>
 </file>
@@ -1819,9 +2017,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,11 +2596,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R171"/>
+  <dimension ref="A1:R203"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B171" sqref="B171"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5466,6 +5664,646 @@
         <v>13</v>
       </c>
     </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172" t="s">
+        <v>472</v>
+      </c>
+      <c r="C172" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D172">
+        <v>54960</v>
+      </c>
+      <c r="E172" t="s">
+        <v>44</v>
+      </c>
+      <c r="G172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173" t="s">
+        <v>474</v>
+      </c>
+      <c r="C173" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="D173">
+        <v>54090</v>
+      </c>
+      <c r="E173" t="s">
+        <v>44</v>
+      </c>
+      <c r="G173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174" t="s">
+        <v>476</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="D174">
+        <v>54290</v>
+      </c>
+      <c r="E174" t="s">
+        <v>12</v>
+      </c>
+      <c r="G174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175" t="s">
+        <v>478</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="D175">
+        <v>54170</v>
+      </c>
+      <c r="E175" t="s">
+        <v>12</v>
+      </c>
+      <c r="G175">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176" t="s">
+        <v>480</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="D176">
+        <v>54260</v>
+      </c>
+      <c r="E176" t="s">
+        <v>12</v>
+      </c>
+      <c r="G176">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177" t="s">
+        <v>482</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="D177">
+        <v>54200</v>
+      </c>
+      <c r="E177" t="s">
+        <v>12</v>
+      </c>
+      <c r="G177">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178" t="s">
+        <v>484</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="D178">
+        <v>54150</v>
+      </c>
+      <c r="E178" t="s">
+        <v>12</v>
+      </c>
+      <c r="G178">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179" t="s">
+        <v>486</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="D179">
+        <v>54030</v>
+      </c>
+      <c r="E179" t="s">
+        <v>44</v>
+      </c>
+      <c r="G179">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180" t="s">
+        <v>488</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="D180">
+        <v>54130</v>
+      </c>
+      <c r="E180" t="s">
+        <v>12</v>
+      </c>
+      <c r="G180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181" t="s">
+        <v>490</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="D181">
+        <v>54050</v>
+      </c>
+      <c r="E181" t="s">
+        <v>44</v>
+      </c>
+      <c r="G181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182" t="s">
+        <v>492</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="D182">
+        <v>54240</v>
+      </c>
+      <c r="E182" t="s">
+        <v>12</v>
+      </c>
+      <c r="G182">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183" t="s">
+        <v>494</v>
+      </c>
+      <c r="C183" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="D183">
+        <v>54210</v>
+      </c>
+      <c r="E183" t="s">
+        <v>12</v>
+      </c>
+      <c r="G183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184" t="s">
+        <v>496</v>
+      </c>
+      <c r="C184" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="D184">
+        <v>54250</v>
+      </c>
+      <c r="E184" t="s">
+        <v>12</v>
+      </c>
+      <c r="G184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185" t="s">
+        <v>498</v>
+      </c>
+      <c r="C185" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="D185">
+        <v>54000</v>
+      </c>
+      <c r="E185" t="s">
+        <v>44</v>
+      </c>
+      <c r="G185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186" t="s">
+        <v>500</v>
+      </c>
+      <c r="C186" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="D186">
+        <v>54190</v>
+      </c>
+      <c r="E186" t="s">
+        <v>12</v>
+      </c>
+      <c r="G186">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187">
+        <v>186</v>
+      </c>
+      <c r="B187" t="s">
+        <v>502</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="D187">
+        <v>54300</v>
+      </c>
+      <c r="E187" t="s">
+        <v>12</v>
+      </c>
+      <c r="G187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>187</v>
+      </c>
+      <c r="B188" t="s">
+        <v>504</v>
+      </c>
+      <c r="C188" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="D188">
+        <v>54010</v>
+      </c>
+      <c r="E188" t="s">
+        <v>537</v>
+      </c>
+      <c r="G188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189">
+        <v>188</v>
+      </c>
+      <c r="B189" t="s">
+        <v>506</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="D189">
+        <v>54160</v>
+      </c>
+      <c r="E189" t="s">
+        <v>12</v>
+      </c>
+      <c r="G189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190">
+        <v>189</v>
+      </c>
+      <c r="B190" t="s">
+        <v>508</v>
+      </c>
+      <c r="C190" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="D190">
+        <v>54270</v>
+      </c>
+      <c r="E190" t="s">
+        <v>12</v>
+      </c>
+      <c r="G190">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191">
+        <v>190</v>
+      </c>
+      <c r="B191" t="s">
+        <v>510</v>
+      </c>
+      <c r="C191" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="D191">
+        <v>54100</v>
+      </c>
+      <c r="E191" t="s">
+        <v>44</v>
+      </c>
+      <c r="G191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192">
+        <v>191</v>
+      </c>
+      <c r="B192" t="s">
+        <v>512</v>
+      </c>
+      <c r="C192" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="D192">
+        <v>54070</v>
+      </c>
+      <c r="E192" t="s">
+        <v>44</v>
+      </c>
+      <c r="G192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193">
+        <v>192</v>
+      </c>
+      <c r="B193" t="s">
+        <v>514</v>
+      </c>
+      <c r="C193" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="D193">
+        <v>54110</v>
+      </c>
+      <c r="E193" t="s">
+        <v>44</v>
+      </c>
+      <c r="G193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194">
+        <v>193</v>
+      </c>
+      <c r="B194" t="s">
+        <v>516</v>
+      </c>
+      <c r="C194" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="D194">
+        <v>54040</v>
+      </c>
+      <c r="E194" t="s">
+        <v>537</v>
+      </c>
+      <c r="G194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>518</v>
+      </c>
+      <c r="C195" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="D195">
+        <v>54310</v>
+      </c>
+      <c r="E195" t="s">
+        <v>12</v>
+      </c>
+      <c r="G195">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>520</v>
+      </c>
+      <c r="C196" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="D196">
+        <v>54020</v>
+      </c>
+      <c r="E196" t="s">
+        <v>12</v>
+      </c>
+      <c r="G196">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>522</v>
+      </c>
+      <c r="C197" s="4" t="s">
+        <v>523</v>
+      </c>
+      <c r="D197">
+        <v>54080</v>
+      </c>
+      <c r="E197" t="s">
+        <v>44</v>
+      </c>
+      <c r="G197">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>524</v>
+      </c>
+      <c r="C198" s="4" t="s">
+        <v>525</v>
+      </c>
+      <c r="D198">
+        <v>54280</v>
+      </c>
+      <c r="E198" t="s">
+        <v>12</v>
+      </c>
+      <c r="G198">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>526</v>
+      </c>
+      <c r="C199" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="D199">
+        <v>54220</v>
+      </c>
+      <c r="E199" t="s">
+        <v>12</v>
+      </c>
+      <c r="G199">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>528</v>
+      </c>
+      <c r="C200" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="D200">
+        <v>54231</v>
+      </c>
+      <c r="E200" t="s">
+        <v>44</v>
+      </c>
+      <c r="G200">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>530</v>
+      </c>
+      <c r="C201" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="D201">
+        <v>54120</v>
+      </c>
+      <c r="E201" t="s">
+        <v>44</v>
+      </c>
+      <c r="G201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>532</v>
+      </c>
+      <c r="C202" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="D202">
+        <v>54140</v>
+      </c>
+      <c r="E202" t="s">
+        <v>12</v>
+      </c>
+      <c r="G202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>534</v>
+      </c>
+      <c r="C203" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="D203">
+        <v>54180</v>
+      </c>
+      <c r="E203" t="s">
+        <v>12</v>
+      </c>
+      <c r="G203">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5473,10 +6311,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5530,11 +6368,25 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>536</v>
+      </c>
       <c r="G4" t="s">
         <v>23</v>
       </c>
       <c r="H4" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>536</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Essex and Hertfordshire locations
</commit_message>
<xml_diff>
--- a/lists/fire-data.xlsx
+++ b/lists/fire-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="699">
   <si>
     <t>name</t>
   </si>
@@ -1630,6 +1630,489 @@
   </si>
   <si>
     <t>Day staffing</t>
+  </si>
+  <si>
+    <t>Station 85 Saffron Walden</t>
+  </si>
+  <si>
+    <t>CB10 1EH</t>
+  </si>
+  <si>
+    <t>Station 84 Newport</t>
+  </si>
+  <si>
+    <t>CB11 3RU</t>
+  </si>
+  <si>
+    <t>Station 83 Stansted</t>
+  </si>
+  <si>
+    <t>CM24 8AE</t>
+  </si>
+  <si>
+    <t>Station 82 Old Harlow</t>
+  </si>
+  <si>
+    <t>CM17 0DR</t>
+  </si>
+  <si>
+    <t>On-call</t>
+  </si>
+  <si>
+    <t>on-call</t>
+  </si>
+  <si>
+    <t>Station 70 Harlow Central</t>
+  </si>
+  <si>
+    <t>CM20 1DU</t>
+  </si>
+  <si>
+    <t>Station 89 Epping</t>
+  </si>
+  <si>
+    <t>CM16 4AF</t>
+  </si>
+  <si>
+    <t>Station 73 Waltham Abbey</t>
+  </si>
+  <si>
+    <t>EN9 1PA</t>
+  </si>
+  <si>
+    <t>Station 72 Loughton</t>
+  </si>
+  <si>
+    <t>IG10 4PE</t>
+  </si>
+  <si>
+    <t>Station 86 Thaxted</t>
+  </si>
+  <si>
+    <t>CM6 2LP</t>
+  </si>
+  <si>
+    <t>Station 87 Dunmow</t>
+  </si>
+  <si>
+    <t>CM6 1DA</t>
+  </si>
+  <si>
+    <t>Station 88 Leaden Roding</t>
+  </si>
+  <si>
+    <t>CM6 1QB</t>
+  </si>
+  <si>
+    <t>Station 71 Ongar</t>
+  </si>
+  <si>
+    <t>CM5 9DT</t>
+  </si>
+  <si>
+    <t>Station 51 Brentwood</t>
+  </si>
+  <si>
+    <t>CM14 4UZ</t>
+  </si>
+  <si>
+    <t>Station 50 Grays</t>
+  </si>
+  <si>
+    <t>RM17 5QS</t>
+  </si>
+  <si>
+    <t>Station 67 Ingatestone</t>
+  </si>
+  <si>
+    <t>CM4 9EY</t>
+  </si>
+  <si>
+    <t>Station 55 Orsett</t>
+  </si>
+  <si>
+    <t>RM16 3DU</t>
+  </si>
+  <si>
+    <t>Station 68 Billericay</t>
+  </si>
+  <si>
+    <t>CM12 9LL</t>
+  </si>
+  <si>
+    <t>Station 52 Basildon</t>
+  </si>
+  <si>
+    <t>SS14 1EH</t>
+  </si>
+  <si>
+    <t>Station 66 Corringham</t>
+  </si>
+  <si>
+    <t>SS17 9BN</t>
+  </si>
+  <si>
+    <t>Station 34 Chelmsford</t>
+  </si>
+  <si>
+    <t>CM1 2QS</t>
+  </si>
+  <si>
+    <t>Station 33 Great Baddow</t>
+  </si>
+  <si>
+    <t>CM2 7EZ</t>
+  </si>
+  <si>
+    <t>Wholetime; on-call</t>
+  </si>
+  <si>
+    <t>Station 69 Wickford</t>
+  </si>
+  <si>
+    <t>SS12 0QG</t>
+  </si>
+  <si>
+    <t>Station 32 South Woodham Ferrers</t>
+  </si>
+  <si>
+    <t>CM3 5XH</t>
+  </si>
+  <si>
+    <t>Station 35 Rayleigh Weir</t>
+  </si>
+  <si>
+    <t>SS7 3TR</t>
+  </si>
+  <si>
+    <t>Station 54 Canvey</t>
+  </si>
+  <si>
+    <t>SS8 0JD</t>
+  </si>
+  <si>
+    <t>Station 47 Hawkwell</t>
+  </si>
+  <si>
+    <t>SS5 4EG</t>
+  </si>
+  <si>
+    <t>Station 31 Leigh</t>
+  </si>
+  <si>
+    <t>SS9 4AA</t>
+  </si>
+  <si>
+    <t>Station 49 Rochford</t>
+  </si>
+  <si>
+    <t>SS4 1BL</t>
+  </si>
+  <si>
+    <t>Station 30 Southend</t>
+  </si>
+  <si>
+    <t>SS2 5PX</t>
+  </si>
+  <si>
+    <t>Station 42 Shoeburyness</t>
+  </si>
+  <si>
+    <t>SS3 9AR</t>
+  </si>
+  <si>
+    <t>Station 43 Burnham-on-Crouch</t>
+  </si>
+  <si>
+    <t>CM0 8DZ</t>
+  </si>
+  <si>
+    <t>Station 46 Maldon</t>
+  </si>
+  <si>
+    <t>CM9 6SH</t>
+  </si>
+  <si>
+    <t>Station 44 Tillingham</t>
+  </si>
+  <si>
+    <t>CM0 7SQ</t>
+  </si>
+  <si>
+    <t>Station 45 Tollesbury</t>
+  </si>
+  <si>
+    <t>CM9 8RG</t>
+  </si>
+  <si>
+    <t>Station 22 West Mersea</t>
+  </si>
+  <si>
+    <t>CO5 8QT</t>
+  </si>
+  <si>
+    <t>Station 20 Brightlingsea</t>
+  </si>
+  <si>
+    <t>CO7 0BP</t>
+  </si>
+  <si>
+    <t>Station 12 Clacton</t>
+  </si>
+  <si>
+    <t>CO16 8DB</t>
+  </si>
+  <si>
+    <t>Station 19 Weeley</t>
+  </si>
+  <si>
+    <t>CO16 9ED</t>
+  </si>
+  <si>
+    <t>Station 25 Witham</t>
+  </si>
+  <si>
+    <t>CM8 1EW</t>
+  </si>
+  <si>
+    <t>Station 23 Tiptree</t>
+  </si>
+  <si>
+    <t>CO5 0SU</t>
+  </si>
+  <si>
+    <t>Station 24 Coggeshal</t>
+  </si>
+  <si>
+    <t>CO6 1SX</t>
+  </si>
+  <si>
+    <t>Station 10 Colchester</t>
+  </si>
+  <si>
+    <t>CO1 1XT</t>
+  </si>
+  <si>
+    <t>Station 21 Wivenhoe</t>
+  </si>
+  <si>
+    <t>CO7 9EU</t>
+  </si>
+  <si>
+    <t>Station 17 Manningtree</t>
+  </si>
+  <si>
+    <t>CO11 1AU</t>
+  </si>
+  <si>
+    <t>Station 11 Dovercourt</t>
+  </si>
+  <si>
+    <t>CO12 4JE</t>
+  </si>
+  <si>
+    <t>Station 78 Braintree</t>
+  </si>
+  <si>
+    <t>CM7 3JD</t>
+  </si>
+  <si>
+    <t>Station 81 Halstead</t>
+  </si>
+  <si>
+    <t>CO9 1EZ</t>
+  </si>
+  <si>
+    <t>Station 80 Sible Hedingham</t>
+  </si>
+  <si>
+    <t>CO9 3NU</t>
+  </si>
+  <si>
+    <t>Station 79 Wethersfield</t>
+  </si>
+  <si>
+    <t>CM7 4BN</t>
+  </si>
+  <si>
+    <t>Station 18 Frinton</t>
+  </si>
+  <si>
+    <t>CO13 9NG</t>
+  </si>
+  <si>
+    <t>Baldock and Letchworth Fire Station</t>
+  </si>
+  <si>
+    <t>Berkhamsted Fire Station</t>
+  </si>
+  <si>
+    <t>Bishops Stortford Fire Station</t>
+  </si>
+  <si>
+    <t>Borehamwood Fire Station</t>
+  </si>
+  <si>
+    <t>Buntingford Fire Station</t>
+  </si>
+  <si>
+    <t>Cheshunt Fire Station</t>
+  </si>
+  <si>
+    <t>Garston Fire Station</t>
+  </si>
+  <si>
+    <t>Harpenden Fire Station</t>
+  </si>
+  <si>
+    <t>Hatfield Fire Station</t>
+  </si>
+  <si>
+    <t>Hemel Hempstead Fire Station</t>
+  </si>
+  <si>
+    <t>Hertford Fire Station</t>
+  </si>
+  <si>
+    <t>Hitchin Fire Station</t>
+  </si>
+  <si>
+    <t>Hoddesdon Fire Station</t>
+  </si>
+  <si>
+    <t>Kings Langley Fire Station</t>
+  </si>
+  <si>
+    <t>Markyate Fire Station</t>
+  </si>
+  <si>
+    <t>Much Hadham Fire Station</t>
+  </si>
+  <si>
+    <t>Potters Bar Fire Station</t>
+  </si>
+  <si>
+    <t>Redbourn Fire Station</t>
+  </si>
+  <si>
+    <t>Rickmansworth Fire Station</t>
+  </si>
+  <si>
+    <t>Royston Fire Station</t>
+  </si>
+  <si>
+    <t>Sawbridgeworth Fire Station</t>
+  </si>
+  <si>
+    <t>St Albans Fire Station</t>
+  </si>
+  <si>
+    <t>Stevenage Fire Station</t>
+  </si>
+  <si>
+    <t>Tring Fire Station</t>
+  </si>
+  <si>
+    <t>Ware Fire Station</t>
+  </si>
+  <si>
+    <t>Watford Fire Station</t>
+  </si>
+  <si>
+    <t>Welwyn Fire Station</t>
+  </si>
+  <si>
+    <t>Welwyn Garden City Fire Station</t>
+  </si>
+  <si>
+    <t>Wheathampstead Fire Station</t>
+  </si>
+  <si>
+    <t>SG7 6EY</t>
+  </si>
+  <si>
+    <t>HP4 2DW</t>
+  </si>
+  <si>
+    <t>CM23 2PY</t>
+  </si>
+  <si>
+    <t>WD6 1JP</t>
+  </si>
+  <si>
+    <t>SG9 9HU</t>
+  </si>
+  <si>
+    <t>EN8 9LT</t>
+  </si>
+  <si>
+    <t>WD24 5RX</t>
+  </si>
+  <si>
+    <t>AL5 2HU</t>
+  </si>
+  <si>
+    <t>AL10 0DA</t>
+  </si>
+  <si>
+    <t>HP2 5HA</t>
+  </si>
+  <si>
+    <t>SG13 7LD</t>
+  </si>
+  <si>
+    <t>SG4 9JR</t>
+  </si>
+  <si>
+    <t>EN11 8JW</t>
+  </si>
+  <si>
+    <t>WD4 8BP</t>
+  </si>
+  <si>
+    <t>AL3 8LF</t>
+  </si>
+  <si>
+    <t>Wholetime &amp; on-call</t>
+  </si>
+  <si>
+    <t>SG10 6DF</t>
+  </si>
+  <si>
+    <t>EN6 2HF</t>
+  </si>
+  <si>
+    <t>WD3 1FJ</t>
+  </si>
+  <si>
+    <t>SG8 5BD</t>
+  </si>
+  <si>
+    <t>CM21 9AY</t>
+  </si>
+  <si>
+    <t>AL1 1TQ</t>
+  </si>
+  <si>
+    <t>SG1 1HS</t>
+  </si>
+  <si>
+    <t>HP23 5ED</t>
+  </si>
+  <si>
+    <t>SG12 9DR</t>
+  </si>
+  <si>
+    <t>WD17 2AG</t>
+  </si>
+  <si>
+    <t>AL6 9EP</t>
+  </si>
+  <si>
+    <t>AL4 8AY</t>
+  </si>
+  <si>
+    <t>AL7 1LP</t>
   </si>
 </sst>
 </file>
@@ -2017,9 +2500,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection activeCell="B249" sqref="B249"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2596,11 +3080,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R203"/>
+  <dimension ref="A1:R282"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B46" sqref="B46"/>
+      <selection pane="bottomLeft" activeCell="G282" sqref="G254:G282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6304,17 +6789,1295 @@
         <v>3</v>
       </c>
     </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>538</v>
+      </c>
+      <c r="C204" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="E204" t="s">
+        <v>546</v>
+      </c>
+      <c r="G204">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
+        <v>540</v>
+      </c>
+      <c r="C205" t="s">
+        <v>541</v>
+      </c>
+      <c r="E205" t="s">
+        <v>546</v>
+      </c>
+      <c r="G205">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>542</v>
+      </c>
+      <c r="C206" t="s">
+        <v>543</v>
+      </c>
+      <c r="G206">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>544</v>
+      </c>
+      <c r="C207" t="s">
+        <v>545</v>
+      </c>
+      <c r="E207" t="s">
+        <v>546</v>
+      </c>
+      <c r="G207">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>548</v>
+      </c>
+      <c r="C208" t="s">
+        <v>549</v>
+      </c>
+      <c r="E208" t="s">
+        <v>44</v>
+      </c>
+      <c r="G208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>550</v>
+      </c>
+      <c r="C209" t="s">
+        <v>551</v>
+      </c>
+      <c r="G209">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>552</v>
+      </c>
+      <c r="C210" t="s">
+        <v>553</v>
+      </c>
+      <c r="E210" t="s">
+        <v>537</v>
+      </c>
+      <c r="G210">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>554</v>
+      </c>
+      <c r="C211" t="s">
+        <v>555</v>
+      </c>
+      <c r="E211" t="s">
+        <v>44</v>
+      </c>
+      <c r="G211">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212">
+        <v>211</v>
+      </c>
+      <c r="B212" t="s">
+        <v>556</v>
+      </c>
+      <c r="C212" t="s">
+        <v>557</v>
+      </c>
+      <c r="G212">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213">
+        <v>212</v>
+      </c>
+      <c r="B213" t="s">
+        <v>558</v>
+      </c>
+      <c r="C213" t="s">
+        <v>559</v>
+      </c>
+      <c r="G213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214">
+        <v>213</v>
+      </c>
+      <c r="B214" t="s">
+        <v>560</v>
+      </c>
+      <c r="C214" t="s">
+        <v>561</v>
+      </c>
+      <c r="G214">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215">
+        <v>214</v>
+      </c>
+      <c r="B215" t="s">
+        <v>562</v>
+      </c>
+      <c r="C215" t="s">
+        <v>563</v>
+      </c>
+      <c r="G215">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>215</v>
+      </c>
+      <c r="B216" t="s">
+        <v>564</v>
+      </c>
+      <c r="C216" t="s">
+        <v>565</v>
+      </c>
+      <c r="E216" t="s">
+        <v>582</v>
+      </c>
+      <c r="G216">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217">
+        <v>216</v>
+      </c>
+      <c r="B217" t="s">
+        <v>566</v>
+      </c>
+      <c r="C217" t="s">
+        <v>567</v>
+      </c>
+      <c r="E217" t="s">
+        <v>44</v>
+      </c>
+      <c r="G217">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218">
+        <v>217</v>
+      </c>
+      <c r="B218" t="s">
+        <v>568</v>
+      </c>
+      <c r="C218" t="s">
+        <v>569</v>
+      </c>
+      <c r="G218">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219">
+        <v>218</v>
+      </c>
+      <c r="B219" t="s">
+        <v>570</v>
+      </c>
+      <c r="C219" t="s">
+        <v>571</v>
+      </c>
+      <c r="E219" t="s">
+        <v>44</v>
+      </c>
+      <c r="G219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220">
+        <v>219</v>
+      </c>
+      <c r="B220" t="s">
+        <v>572</v>
+      </c>
+      <c r="C220" t="s">
+        <v>573</v>
+      </c>
+      <c r="E220" t="s">
+        <v>546</v>
+      </c>
+      <c r="G220">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221">
+        <v>220</v>
+      </c>
+      <c r="B221" t="s">
+        <v>574</v>
+      </c>
+      <c r="C221" t="s">
+        <v>575</v>
+      </c>
+      <c r="E221" t="s">
+        <v>44</v>
+      </c>
+      <c r="G221">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222">
+        <v>221</v>
+      </c>
+      <c r="B222" t="s">
+        <v>576</v>
+      </c>
+      <c r="C222" t="s">
+        <v>577</v>
+      </c>
+      <c r="G222">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>222</v>
+      </c>
+      <c r="B223" t="s">
+        <v>578</v>
+      </c>
+      <c r="C223" t="s">
+        <v>579</v>
+      </c>
+      <c r="E223" t="s">
+        <v>44</v>
+      </c>
+      <c r="G223">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224">
+        <v>223</v>
+      </c>
+      <c r="B224" t="s">
+        <v>580</v>
+      </c>
+      <c r="C224" t="s">
+        <v>581</v>
+      </c>
+      <c r="E224" t="s">
+        <v>537</v>
+      </c>
+      <c r="G224">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225">
+        <v>224</v>
+      </c>
+      <c r="B225" t="s">
+        <v>583</v>
+      </c>
+      <c r="C225" t="s">
+        <v>584</v>
+      </c>
+      <c r="G225">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A226">
+        <v>225</v>
+      </c>
+      <c r="B226" t="s">
+        <v>585</v>
+      </c>
+      <c r="C226" t="s">
+        <v>586</v>
+      </c>
+      <c r="E226" t="s">
+        <v>537</v>
+      </c>
+      <c r="G226">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A227">
+        <v>226</v>
+      </c>
+      <c r="B227" t="s">
+        <v>587</v>
+      </c>
+      <c r="C227" t="s">
+        <v>588</v>
+      </c>
+      <c r="E227" t="s">
+        <v>44</v>
+      </c>
+      <c r="G227">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A228">
+        <v>227</v>
+      </c>
+      <c r="B228" t="s">
+        <v>589</v>
+      </c>
+      <c r="C228" t="s">
+        <v>590</v>
+      </c>
+      <c r="G228">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229">
+        <v>228</v>
+      </c>
+      <c r="B229" t="s">
+        <v>591</v>
+      </c>
+      <c r="C229" t="s">
+        <v>592</v>
+      </c>
+      <c r="E229" t="s">
+        <v>546</v>
+      </c>
+      <c r="G229">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>229</v>
+      </c>
+      <c r="B230" t="s">
+        <v>593</v>
+      </c>
+      <c r="C230" t="s">
+        <v>594</v>
+      </c>
+      <c r="E230" t="s">
+        <v>44</v>
+      </c>
+      <c r="G230">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231">
+        <v>230</v>
+      </c>
+      <c r="B231" t="s">
+        <v>595</v>
+      </c>
+      <c r="C231" t="s">
+        <v>596</v>
+      </c>
+      <c r="E231" t="s">
+        <v>546</v>
+      </c>
+      <c r="G231">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232">
+        <v>231</v>
+      </c>
+      <c r="B232" t="s">
+        <v>597</v>
+      </c>
+      <c r="C232" t="s">
+        <v>598</v>
+      </c>
+      <c r="E232" t="s">
+        <v>44</v>
+      </c>
+      <c r="G232">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233">
+        <v>232</v>
+      </c>
+      <c r="B233" t="s">
+        <v>599</v>
+      </c>
+      <c r="C233" t="s">
+        <v>600</v>
+      </c>
+      <c r="G233">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234">
+        <v>233</v>
+      </c>
+      <c r="B234" t="s">
+        <v>601</v>
+      </c>
+      <c r="C234" t="s">
+        <v>602</v>
+      </c>
+      <c r="G234">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235">
+        <v>234</v>
+      </c>
+      <c r="B235" t="s">
+        <v>603</v>
+      </c>
+      <c r="C235" t="s">
+        <v>604</v>
+      </c>
+      <c r="G235">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236">
+        <v>235</v>
+      </c>
+      <c r="B236" t="s">
+        <v>605</v>
+      </c>
+      <c r="C236" t="s">
+        <v>606</v>
+      </c>
+      <c r="G236">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>236</v>
+      </c>
+      <c r="B237" t="s">
+        <v>607</v>
+      </c>
+      <c r="C237" t="s">
+        <v>608</v>
+      </c>
+      <c r="G237">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238">
+        <v>237</v>
+      </c>
+      <c r="B238" t="s">
+        <v>609</v>
+      </c>
+      <c r="C238" t="s">
+        <v>610</v>
+      </c>
+      <c r="E238" t="s">
+        <v>546</v>
+      </c>
+      <c r="G238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>238</v>
+      </c>
+      <c r="B239" t="s">
+        <v>611</v>
+      </c>
+      <c r="C239" t="s">
+        <v>612</v>
+      </c>
+      <c r="E239" t="s">
+        <v>546</v>
+      </c>
+      <c r="G239">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>239</v>
+      </c>
+      <c r="B240" t="s">
+        <v>613</v>
+      </c>
+      <c r="C240" t="s">
+        <v>614</v>
+      </c>
+      <c r="G240">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>240</v>
+      </c>
+      <c r="B241" t="s">
+        <v>615</v>
+      </c>
+      <c r="C241" t="s">
+        <v>616</v>
+      </c>
+      <c r="E241" t="s">
+        <v>546</v>
+      </c>
+      <c r="G241">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>241</v>
+      </c>
+      <c r="B242" t="s">
+        <v>617</v>
+      </c>
+      <c r="C242" t="s">
+        <v>618</v>
+      </c>
+      <c r="G242">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243">
+        <v>242</v>
+      </c>
+      <c r="B243" t="s">
+        <v>619</v>
+      </c>
+      <c r="C243" t="s">
+        <v>620</v>
+      </c>
+      <c r="G243">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>243</v>
+      </c>
+      <c r="B244" t="s">
+        <v>621</v>
+      </c>
+      <c r="C244" t="s">
+        <v>622</v>
+      </c>
+      <c r="G244">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245">
+        <v>244</v>
+      </c>
+      <c r="B245" t="s">
+        <v>623</v>
+      </c>
+      <c r="C245" t="s">
+        <v>624</v>
+      </c>
+      <c r="E245" t="s">
+        <v>44</v>
+      </c>
+      <c r="G245">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246">
+        <v>245</v>
+      </c>
+      <c r="B246" t="s">
+        <v>625</v>
+      </c>
+      <c r="C246" t="s">
+        <v>626</v>
+      </c>
+      <c r="E246" t="s">
+        <v>546</v>
+      </c>
+      <c r="G246">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247">
+        <v>246</v>
+      </c>
+      <c r="B247" t="s">
+        <v>627</v>
+      </c>
+      <c r="C247" t="s">
+        <v>628</v>
+      </c>
+      <c r="E247" t="s">
+        <v>546</v>
+      </c>
+      <c r="G247">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248">
+        <v>247</v>
+      </c>
+      <c r="B248" t="s">
+        <v>629</v>
+      </c>
+      <c r="C248" t="s">
+        <v>630</v>
+      </c>
+      <c r="E248" t="s">
+        <v>537</v>
+      </c>
+      <c r="G248">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249">
+        <v>248</v>
+      </c>
+      <c r="B249" t="s">
+        <v>631</v>
+      </c>
+      <c r="C249" t="s">
+        <v>632</v>
+      </c>
+      <c r="E249" t="s">
+        <v>546</v>
+      </c>
+      <c r="G249">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250">
+        <v>249</v>
+      </c>
+      <c r="B250" t="s">
+        <v>633</v>
+      </c>
+      <c r="C250" t="s">
+        <v>634</v>
+      </c>
+      <c r="G250">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>250</v>
+      </c>
+      <c r="B251" t="s">
+        <v>635</v>
+      </c>
+      <c r="C251" t="s">
+        <v>636</v>
+      </c>
+      <c r="G251">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252">
+        <v>251</v>
+      </c>
+      <c r="B252" t="s">
+        <v>637</v>
+      </c>
+      <c r="C252" t="s">
+        <v>638</v>
+      </c>
+      <c r="G252">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253">
+        <v>252</v>
+      </c>
+      <c r="B253" t="s">
+        <v>639</v>
+      </c>
+      <c r="C253" t="s">
+        <v>640</v>
+      </c>
+      <c r="E253" t="s">
+        <v>546</v>
+      </c>
+      <c r="G253">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254">
+        <v>253</v>
+      </c>
+      <c r="B254" t="s">
+        <v>641</v>
+      </c>
+      <c r="C254" t="s">
+        <v>670</v>
+      </c>
+      <c r="E254" t="s">
+        <v>685</v>
+      </c>
+      <c r="G254">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255">
+        <v>254</v>
+      </c>
+      <c r="B255" t="s">
+        <v>642</v>
+      </c>
+      <c r="C255" t="s">
+        <v>671</v>
+      </c>
+      <c r="E255" t="s">
+        <v>547</v>
+      </c>
+      <c r="G255">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256">
+        <v>255</v>
+      </c>
+      <c r="B256" t="s">
+        <v>643</v>
+      </c>
+      <c r="C256" t="s">
+        <v>672</v>
+      </c>
+      <c r="E256" t="s">
+        <v>685</v>
+      </c>
+      <c r="G256">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257">
+        <v>256</v>
+      </c>
+      <c r="B257" t="s">
+        <v>644</v>
+      </c>
+      <c r="C257" t="s">
+        <v>673</v>
+      </c>
+      <c r="E257" t="s">
+        <v>44</v>
+      </c>
+      <c r="G257">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>257</v>
+      </c>
+      <c r="B258" t="s">
+        <v>645</v>
+      </c>
+      <c r="C258" t="s">
+        <v>674</v>
+      </c>
+      <c r="E258" t="s">
+        <v>547</v>
+      </c>
+      <c r="G258">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259">
+        <v>258</v>
+      </c>
+      <c r="B259" t="s">
+        <v>646</v>
+      </c>
+      <c r="C259" t="s">
+        <v>675</v>
+      </c>
+      <c r="E259" t="s">
+        <v>685</v>
+      </c>
+      <c r="G259">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260">
+        <v>259</v>
+      </c>
+      <c r="B260" t="s">
+        <v>647</v>
+      </c>
+      <c r="C260" t="s">
+        <v>676</v>
+      </c>
+      <c r="E260" t="s">
+        <v>44</v>
+      </c>
+      <c r="G260">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261">
+        <v>260</v>
+      </c>
+      <c r="B261" t="s">
+        <v>648</v>
+      </c>
+      <c r="C261" t="s">
+        <v>677</v>
+      </c>
+      <c r="E261" t="s">
+        <v>547</v>
+      </c>
+      <c r="G261">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262">
+        <v>261</v>
+      </c>
+      <c r="B262" t="s">
+        <v>649</v>
+      </c>
+      <c r="C262" t="s">
+        <v>678</v>
+      </c>
+      <c r="E262" t="s">
+        <v>685</v>
+      </c>
+      <c r="G262">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263">
+        <v>262</v>
+      </c>
+      <c r="B263" t="s">
+        <v>650</v>
+      </c>
+      <c r="C263" t="s">
+        <v>679</v>
+      </c>
+      <c r="E263" t="s">
+        <v>44</v>
+      </c>
+      <c r="G263">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264">
+        <v>263</v>
+      </c>
+      <c r="B264" t="s">
+        <v>651</v>
+      </c>
+      <c r="C264" t="s">
+        <v>680</v>
+      </c>
+      <c r="E264" t="s">
+        <v>685</v>
+      </c>
+      <c r="G264">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>264</v>
+      </c>
+      <c r="B265" t="s">
+        <v>652</v>
+      </c>
+      <c r="C265" t="s">
+        <v>681</v>
+      </c>
+      <c r="E265" t="s">
+        <v>685</v>
+      </c>
+      <c r="G265">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266">
+        <v>265</v>
+      </c>
+      <c r="B266" t="s">
+        <v>653</v>
+      </c>
+      <c r="C266" t="s">
+        <v>682</v>
+      </c>
+      <c r="E266" t="s">
+        <v>547</v>
+      </c>
+      <c r="G266">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267">
+        <v>266</v>
+      </c>
+      <c r="B267" t="s">
+        <v>654</v>
+      </c>
+      <c r="C267" t="s">
+        <v>683</v>
+      </c>
+      <c r="E267" t="s">
+        <v>547</v>
+      </c>
+      <c r="G267">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268">
+        <v>267</v>
+      </c>
+      <c r="B268" t="s">
+        <v>655</v>
+      </c>
+      <c r="C268" t="s">
+        <v>684</v>
+      </c>
+      <c r="E268" t="s">
+        <v>547</v>
+      </c>
+      <c r="G268">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269">
+        <v>268</v>
+      </c>
+      <c r="B269" t="s">
+        <v>656</v>
+      </c>
+      <c r="C269" t="s">
+        <v>686</v>
+      </c>
+      <c r="E269" t="s">
+        <v>547</v>
+      </c>
+      <c r="G269">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270">
+        <v>269</v>
+      </c>
+      <c r="B270" t="s">
+        <v>657</v>
+      </c>
+      <c r="C270" t="s">
+        <v>687</v>
+      </c>
+      <c r="E270" t="s">
+        <v>685</v>
+      </c>
+      <c r="G270">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271">
+        <v>270</v>
+      </c>
+      <c r="B271" t="s">
+        <v>658</v>
+      </c>
+      <c r="C271" t="s">
+        <v>687</v>
+      </c>
+      <c r="E271" t="s">
+        <v>547</v>
+      </c>
+      <c r="G271">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>271</v>
+      </c>
+      <c r="B272" t="s">
+        <v>659</v>
+      </c>
+      <c r="C272" t="s">
+        <v>688</v>
+      </c>
+      <c r="E272" t="s">
+        <v>44</v>
+      </c>
+      <c r="G272">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273">
+        <v>272</v>
+      </c>
+      <c r="B273" t="s">
+        <v>660</v>
+      </c>
+      <c r="C273" t="s">
+        <v>689</v>
+      </c>
+      <c r="E273" t="s">
+        <v>44</v>
+      </c>
+      <c r="G273">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274">
+        <v>273</v>
+      </c>
+      <c r="B274" t="s">
+        <v>661</v>
+      </c>
+      <c r="C274" t="s">
+        <v>690</v>
+      </c>
+      <c r="E274" t="s">
+        <v>547</v>
+      </c>
+      <c r="G274">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>274</v>
+      </c>
+      <c r="B275" t="s">
+        <v>662</v>
+      </c>
+      <c r="C275" t="s">
+        <v>691</v>
+      </c>
+      <c r="E275" t="s">
+        <v>44</v>
+      </c>
+      <c r="G275">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>275</v>
+      </c>
+      <c r="B276" t="s">
+        <v>663</v>
+      </c>
+      <c r="C276" t="s">
+        <v>692</v>
+      </c>
+      <c r="E276" t="s">
+        <v>44</v>
+      </c>
+      <c r="G276">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>276</v>
+      </c>
+      <c r="B277" t="s">
+        <v>664</v>
+      </c>
+      <c r="C277" t="s">
+        <v>693</v>
+      </c>
+      <c r="E277" t="s">
+        <v>547</v>
+      </c>
+      <c r="G277">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>277</v>
+      </c>
+      <c r="B278" t="s">
+        <v>665</v>
+      </c>
+      <c r="C278" t="s">
+        <v>694</v>
+      </c>
+      <c r="E278" t="s">
+        <v>547</v>
+      </c>
+      <c r="G278">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>278</v>
+      </c>
+      <c r="B279" t="s">
+        <v>666</v>
+      </c>
+      <c r="C279" t="s">
+        <v>695</v>
+      </c>
+      <c r="E279" t="s">
+        <v>44</v>
+      </c>
+      <c r="G279">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>279</v>
+      </c>
+      <c r="B280" t="s">
+        <v>667</v>
+      </c>
+      <c r="C280" t="s">
+        <v>696</v>
+      </c>
+      <c r="E280" t="s">
+        <v>547</v>
+      </c>
+      <c r="G280">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>280</v>
+      </c>
+      <c r="B281" t="s">
+        <v>668</v>
+      </c>
+      <c r="C281" t="s">
+        <v>698</v>
+      </c>
+      <c r="E281" t="s">
+        <v>685</v>
+      </c>
+      <c r="G281">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>281</v>
+      </c>
+      <c r="B282" t="s">
+        <v>669</v>
+      </c>
+      <c r="C282" t="s">
+        <v>697</v>
+      </c>
+      <c r="E282" t="s">
+        <v>547</v>
+      </c>
+      <c r="G282">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6382,11 +8145,25 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>547</v>
+      </c>
       <c r="G5" t="s">
         <v>536</v>
       </c>
       <c r="H5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>547</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>